<commit_message>
almost done - have to add the piece that adds from the wall lists
</commit_message>
<xml_diff>
--- a/AdventOfCode2017Day3/notes/Part2Breakdown.xlsx
+++ b/AdventOfCode2017Day3/notes/Part2Breakdown.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\source\repos\AdventOfCode2017Day3\AdventOfCode2017Day3\notes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Source\Repos\aoc2017-prob3\AdventOfCode2017Day3\notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1B4D9B-C90E-44D0-B903-D40F10667DA9}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1733CD87-3AEC-415E-958D-988A9D06CE21}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12855" windowHeight="14265" xr2:uid="{28CF73D2-14E5-442D-9F8C-5BCEAC395656}"/>
   </bookViews>
@@ -24,8 +24,43 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Thomas Tatum</author>
+  </authors>
+  <commentList>
+    <comment ref="T3" authorId="0" shapeId="0" xr:uid="{2DC0934C-4E6A-411A-B08C-1E8CB3C7D342}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thomas Tatum:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Skip this row - hard code the values
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="55">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -87,20 +122,116 @@
     <t>na</t>
   </si>
   <si>
-    <t>which wall add the value?</t>
-  </si>
-  <si>
     <t>new wall with single value</t>
   </si>
   <si>
     <t xml:space="preserve"> n</t>
+  </si>
+  <si>
+    <t>push value to wall</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> e</t>
+  </si>
+  <si>
+    <t>WALL ARRAY</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>10,5</t>
+  </si>
+  <si>
+    <t>10,1,1</t>
+  </si>
+  <si>
+    <t>11,10,5</t>
+  </si>
+  <si>
+    <t>11N</t>
+  </si>
+  <si>
+    <t>11,23</t>
+  </si>
+  <si>
+    <t>11,23,25</t>
+  </si>
+  <si>
+    <t>11,23,25,26</t>
+  </si>
+  <si>
+    <t>26,54</t>
+  </si>
+  <si>
+    <t>26,54,57</t>
+  </si>
+  <si>
+    <t>5,4,2,57</t>
+  </si>
+  <si>
+    <t>26,54,57,59</t>
+  </si>
+  <si>
+    <t>26N</t>
+  </si>
+  <si>
+    <t>59N</t>
+  </si>
+  <si>
+    <t>59.122.133.</t>
+  </si>
+  <si>
+    <t>11,10,5,142</t>
+  </si>
+  <si>
+    <t>304,147,</t>
+  </si>
+  <si>
+    <t>362,747,806,</t>
+  </si>
+  <si>
+    <t>362,747,806,880</t>
+  </si>
+  <si>
+    <t>362,747,806,880,931</t>
+  </si>
+  <si>
+    <t>362,747,806,880,931,957</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>5,4,2</t>
+  </si>
+  <si>
+    <t>351,11,23,25,26</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>931,26,54,57,59</t>
+  </si>
+  <si>
+    <t>25,1,2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,8 +253,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -140,8 +298,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -149,13 +317,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,11 +368,34 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="4" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -185,6 +408,101 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6566862" cy="1125693"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE16420A-3B88-4D05-8225-C2BB1E77D4D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11363325" y="5743575"/>
+          <a:ext cx="6566862" cy="1125693"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Here is the</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> pattern for array building:  We have 3 wall types - 0..n-1, n-1 and n</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>We will call them normal, nexttolast and last.  These refer to the position on the wall.  </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>If we are normal, we push it onto the end of the array</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>if we are nexttolast, we push the value at end of the array and add to beginning of the next directions last array</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>If we are last, we push at the end and then create a new next array with only the new values</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -483,19 +801,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E55E8-39C0-4439-85C5-5B4B47E456D6}">
-  <dimension ref="B1:AA54"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972E55E8-39C0-4439-85C5-5B4B47E456D6}">
+  <dimension ref="B1:AH54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P44" sqref="P44"/>
+    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <pane xSplit="15" ySplit="19" topLeftCell="P20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="P1" sqref="P1"/>
+      <selection pane="bottomLeft" activeCell="A20" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="14" max="27" width="9.140625" style="1"/>
+    <col min="1" max="1" width="5.140625" customWidth="1"/>
+    <col min="14" max="19" width="9.140625" style="1"/>
+    <col min="20" max="20" width="28.28515625" style="9" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -532,14 +860,18 @@
       <c r="M1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U1" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -550,19 +882,61 @@
         <v>19</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="1">
+        <v>6591</v>
+      </c>
+      <c r="AA2" s="1">
+        <v>6444</v>
+      </c>
+      <c r="AB2" s="1">
+        <v>6155</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>5733</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>5336</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>5022</v>
+      </c>
+      <c r="AF2" s="1">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="3" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>2</v>
       </c>
@@ -587,7 +961,7 @@
         <v>18</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>0</v>
@@ -595,8 +969,39 @@
       <c r="Q3" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T3" s="11">
+        <v>11</v>
+      </c>
+      <c r="U3" s="12">
+        <v>1</v>
+      </c>
+      <c r="V3" s="12">
+        <v>11</v>
+      </c>
+      <c r="W3" s="12"/>
+      <c r="Z3" s="1">
+        <v>13486</v>
+      </c>
+      <c r="AA3" s="1">
+        <v>147</v>
+      </c>
+      <c r="AB3" s="1">
+        <v>142</v>
+      </c>
+      <c r="AC3" s="1">
+        <v>133</v>
+      </c>
+      <c r="AD3" s="1">
+        <v>122</v>
+      </c>
+      <c r="AE3" s="1">
+        <v>59</v>
+      </c>
+      <c r="AF3" s="1">
+        <v>2391</v>
+      </c>
+    </row>
+    <row r="4" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>3</v>
       </c>
@@ -621,10 +1026,40 @@
         <v>17</v>
       </c>
       <c r="O4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="U4" s="1">
+        <v>21</v>
+      </c>
+      <c r="V4" s="1">
+        <v>2</v>
+      </c>
+      <c r="Z4" s="1">
+        <v>14267</v>
+      </c>
+      <c r="AA4" s="1">
+        <v>304</v>
+      </c>
+      <c r="AB4" s="1">
+        <v>5</v>
+      </c>
+      <c r="AC4" s="1">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="1">
+        <v>2</v>
+      </c>
+      <c r="AE4" s="1">
+        <v>57</v>
+      </c>
+      <c r="AF4" s="1">
+        <v>2275</v>
+      </c>
+    </row>
+    <row r="5" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>4</v>
       </c>
@@ -648,8 +1083,35 @@
       <c r="N5" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="V5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>15252</v>
+      </c>
+      <c r="AA5" s="1">
+        <v>330</v>
+      </c>
+      <c r="AB5" s="1">
+        <v>10</v>
+      </c>
+      <c r="AC5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="1">
+        <v>54</v>
+      </c>
+      <c r="AF5" s="1">
+        <v>2105</v>
+      </c>
+    </row>
+    <row r="6" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>5</v>
       </c>
@@ -679,8 +1141,38 @@
       <c r="Q6" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="W6" s="1">
+        <v>5</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>16295</v>
+      </c>
+      <c r="AA6" s="1">
+        <v>351</v>
+      </c>
+      <c r="AB6" s="1">
+        <v>11</v>
+      </c>
+      <c r="AC6" s="1">
+        <v>23</v>
+      </c>
+      <c r="AD6" s="1">
+        <v>25</v>
+      </c>
+      <c r="AE6" s="1">
+        <v>26</v>
+      </c>
+      <c r="AF6" s="1">
+        <v>1968</v>
+      </c>
+    </row>
+    <row r="7" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>6</v>
       </c>
@@ -707,8 +1199,38 @@
       <c r="O7" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="W7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>17008</v>
+      </c>
+      <c r="AA7" s="1">
+        <v>362</v>
+      </c>
+      <c r="AB7" s="1">
+        <v>747</v>
+      </c>
+      <c r="AC7" s="1">
+        <v>806</v>
+      </c>
+      <c r="AD7" s="1">
+        <v>880</v>
+      </c>
+      <c r="AE7" s="1">
+        <v>931</v>
+      </c>
+      <c r="AF7" s="1">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="8" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>7</v>
       </c>
@@ -738,8 +1260,17 @@
       <c r="Q8" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="S8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>8</v>
       </c>
@@ -766,8 +1297,11 @@
       <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T9" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>9</v>
       </c>
@@ -794,8 +1328,17 @@
       <c r="O10" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AH10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>10</v>
       </c>
@@ -825,8 +1368,20 @@
       <c r="Q11" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T11" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG11">
+        <v>1</v>
+      </c>
+      <c r="AH11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>11</v>
       </c>
@@ -853,8 +1408,11 @@
       <c r="N12" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>12</v>
       </c>
@@ -881,8 +1439,14 @@
       <c r="O13" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>13</v>
       </c>
@@ -912,8 +1476,14 @@
       <c r="Q14" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="U14" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>14</v>
       </c>
@@ -940,8 +1510,11 @@
       <c r="N15" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="V15" s="7">
+        <v>59122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:34" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>15</v>
       </c>
@@ -968,8 +1541,11 @@
       <c r="N16" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V16" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>16</v>
       </c>
@@ -996,8 +1572,14 @@
       <c r="O17" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V17" s="7">
+        <v>59122133142</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>17</v>
       </c>
@@ -1027,8 +1609,14 @@
       <c r="Q18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="V18" s="7">
+        <v>59122133142147</v>
+      </c>
+      <c r="W18" s="1">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>18</v>
       </c>
@@ -1058,8 +1646,11 @@
       <c r="N19" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W19" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>19</v>
       </c>
@@ -1086,8 +1677,11 @@
       <c r="N20" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="21" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="W20" s="7">
+        <v>330304147</v>
+      </c>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>20</v>
       </c>
@@ -1114,8 +1708,14 @@
       <c r="O21" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T21" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="W21" s="7">
+        <v>351304330147</v>
+      </c>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B22">
         <v>21</v>
       </c>
@@ -1145,8 +1745,14 @@
       <c r="Q22" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="23" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T22" s="9">
+        <v>362</v>
+      </c>
+      <c r="W22" s="7">
+        <v>362351304330147</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>22</v>
       </c>
@@ -1173,8 +1779,11 @@
       <c r="N23" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="24" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T23" s="9">
+        <v>362747</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>23</v>
       </c>
@@ -1201,29 +1810,11 @@
       <c r="N24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R24" s="1">
-        <v>6591</v>
-      </c>
-      <c r="S24" s="1">
-        <v>6444</v>
-      </c>
-      <c r="T24" s="1">
-        <v>6155</v>
-      </c>
-      <c r="U24" s="1">
-        <v>5733</v>
-      </c>
-      <c r="V24" s="1">
-        <v>5336</v>
-      </c>
-      <c r="W24" s="1">
-        <v>5022</v>
-      </c>
-      <c r="X24" s="1">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="25" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T24" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>24</v>
       </c>
@@ -1250,29 +1841,11 @@
       <c r="N25" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="R25" s="1">
-        <v>13486</v>
-      </c>
-      <c r="S25" s="1">
-        <v>147</v>
-      </c>
-      <c r="T25" s="1">
-        <v>142</v>
-      </c>
-      <c r="U25" s="1">
-        <v>133</v>
-      </c>
-      <c r="V25" s="1">
-        <v>122</v>
-      </c>
-      <c r="W25" s="1">
-        <v>59</v>
-      </c>
-      <c r="X25" s="1">
-        <v>2391</v>
-      </c>
-    </row>
-    <row r="26" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T25" s="9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>25</v>
       </c>
@@ -1299,29 +1872,14 @@
       <c r="O26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R26" s="1">
-        <v>14267</v>
-      </c>
-      <c r="S26" s="1">
-        <v>304</v>
-      </c>
-      <c r="T26" s="1">
-        <v>5</v>
-      </c>
-      <c r="U26" s="1">
-        <v>4</v>
-      </c>
-      <c r="V26" s="1">
-        <v>2</v>
-      </c>
-      <c r="W26" s="1">
-        <v>57</v>
-      </c>
-      <c r="X26" s="1">
-        <v>2275</v>
-      </c>
-    </row>
-    <row r="27" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T26" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="U26" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>26</v>
       </c>
@@ -1351,29 +1909,14 @@
       <c r="Q27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R27" s="1">
-        <v>15252</v>
-      </c>
-      <c r="S27" s="1">
-        <v>330</v>
-      </c>
-      <c r="T27" s="1">
-        <v>10</v>
-      </c>
-      <c r="U27" s="2">
-        <v>1</v>
-      </c>
-      <c r="V27" s="3">
-        <v>1</v>
-      </c>
-      <c r="W27" s="1">
-        <v>54</v>
-      </c>
-      <c r="X27" s="1">
-        <v>2105</v>
-      </c>
-    </row>
-    <row r="28" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="T27" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U27" s="1">
+        <v>957</v>
+      </c>
+    </row>
+    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>27</v>
       </c>
@@ -1400,29 +1943,8 @@
       <c r="N28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R28" s="1">
-        <v>16295</v>
-      </c>
-      <c r="S28" s="1">
-        <v>351</v>
-      </c>
-      <c r="T28" s="1">
-        <v>11</v>
-      </c>
-      <c r="U28" s="1">
-        <v>23</v>
-      </c>
-      <c r="V28" s="1">
-        <v>25</v>
-      </c>
-      <c r="W28" s="1">
-        <v>26</v>
-      </c>
-      <c r="X28" s="1">
-        <v>1968</v>
-      </c>
-    </row>
-    <row r="29" spans="2:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>28</v>
       </c>
@@ -1449,29 +1971,8 @@
       <c r="N29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R29" s="1">
-        <v>17008</v>
-      </c>
-      <c r="S29" s="1">
-        <v>362</v>
-      </c>
-      <c r="T29" s="1">
-        <v>747</v>
-      </c>
-      <c r="U29" s="1">
-        <v>806</v>
-      </c>
-      <c r="V29" s="1">
-        <v>880</v>
-      </c>
-      <c r="W29" s="1">
-        <v>931</v>
-      </c>
-      <c r="X29" s="1">
-        <v>957</v>
-      </c>
-    </row>
-    <row r="30" spans="2:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>29</v>
       </c>
@@ -1499,7 +2000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>30</v>
       </c>
@@ -1527,7 +2028,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="32" spans="2:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>31</v>
       </c>
@@ -1992,5 +2493,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>